<commit_message>
update OTP episode dataset
</commit_message>
<xml_diff>
--- a/data-raw/cmam/otpEpisode_calculations.xlsx
+++ b/data-raw/cmam/otpEpisode_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ernest/GitHub/squeacr/data-raw/cmam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59185AF9-ED6F-644A-AFE6-61962806CBE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B858DA95-280B-F441-A57F-5E0A012CA035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="74">
   <si>
     <t>index</t>
   </si>
@@ -234,13 +234,7 @@
     <t>Alkareba</t>
   </si>
   <si>
-    <t>Sharg Algazira</t>
-  </si>
-  <si>
     <t>Alganed</t>
-  </si>
-  <si>
-    <t>South Algazira</t>
   </si>
   <si>
     <t>Barakat</t>
@@ -686,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="D362" sqref="D362"/>
+    <sheetView tabSelected="1" topLeftCell="A359" workbookViewId="0">
+      <selection activeCell="L370" sqref="L370:L375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14663,7 +14657,7 @@
         <v>60</v>
       </c>
       <c r="M338" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="339" spans="1:13" x14ac:dyDescent="0.2">
@@ -14699,7 +14693,7 @@
         <v>60</v>
       </c>
       <c r="M339" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="340" spans="1:13" x14ac:dyDescent="0.2">
@@ -15919,11 +15913,11 @@
       <c r="K370" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L370" s="18" t="s">
+      <c r="L370" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="M370" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="M370" s="18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="371" spans="1:13" x14ac:dyDescent="0.2">
@@ -15960,11 +15954,11 @@
       <c r="K371" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L371" s="18" t="s">
+      <c r="L371" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="M371" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="M371" s="18" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="372" spans="1:13" x14ac:dyDescent="0.2">
@@ -16001,11 +15995,11 @@
       <c r="K372" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L372" s="18" t="s">
-        <v>68</v>
+      <c r="L372" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="M372" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="373" spans="1:13" x14ac:dyDescent="0.2">
@@ -16042,11 +16036,11 @@
       <c r="K373" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L373" s="18" t="s">
-        <v>68</v>
+      <c r="L373" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="M373" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="374" spans="1:13" x14ac:dyDescent="0.2">
@@ -16083,11 +16077,11 @@
       <c r="K374" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L374" s="18" t="s">
-        <v>68</v>
+      <c r="L374" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="M374" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="375" spans="1:13" x14ac:dyDescent="0.2">
@@ -16124,11 +16118,11 @@
       <c r="K375" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="L375" s="18" t="s">
-        <v>68</v>
+      <c r="L375" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="M375" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="376" spans="1:13" x14ac:dyDescent="0.2">
@@ -16166,10 +16160,10 @@
         <v>59</v>
       </c>
       <c r="L376" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M376" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="377" spans="1:13" x14ac:dyDescent="0.2">
@@ -16207,10 +16201,10 @@
         <v>59</v>
       </c>
       <c r="L377" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M377" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="378" spans="1:13" x14ac:dyDescent="0.2">
@@ -16248,10 +16242,10 @@
         <v>59</v>
       </c>
       <c r="L378" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M378" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="379" spans="1:13" x14ac:dyDescent="0.2">
@@ -16289,10 +16283,10 @@
         <v>59</v>
       </c>
       <c r="L379" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M379" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="380" spans="1:13" x14ac:dyDescent="0.2">
@@ -16330,10 +16324,10 @@
         <v>59</v>
       </c>
       <c r="L380" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M380" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="381" spans="1:13" x14ac:dyDescent="0.2">
@@ -16371,10 +16365,10 @@
         <v>59</v>
       </c>
       <c r="L381" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M381" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="382" spans="1:13" x14ac:dyDescent="0.2">
@@ -16412,10 +16406,10 @@
         <v>59</v>
       </c>
       <c r="L382" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M382" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="383" spans="1:13" x14ac:dyDescent="0.2">
@@ -16453,10 +16447,10 @@
         <v>59</v>
       </c>
       <c r="L383" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M383" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="384" spans="1:13" x14ac:dyDescent="0.2">
@@ -16494,10 +16488,10 @@
         <v>59</v>
       </c>
       <c r="L384" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M384" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="M384" s="18" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="385" spans="1:13" x14ac:dyDescent="0.2">
@@ -16535,10 +16529,10 @@
         <v>59</v>
       </c>
       <c r="L385" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M385" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="M385" s="18" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="386" spans="1:13" x14ac:dyDescent="0.2">
@@ -16576,10 +16570,10 @@
         <v>59</v>
       </c>
       <c r="L386" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M386" s="18" t="s">
         <v>70</v>
-      </c>
-      <c r="M386" s="18" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="387" spans="1:13" x14ac:dyDescent="0.2">
@@ -16617,10 +16611,10 @@
         <v>59</v>
       </c>
       <c r="L387" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M387" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="388" spans="1:13" x14ac:dyDescent="0.2">
@@ -16658,10 +16652,10 @@
         <v>59</v>
       </c>
       <c r="L388" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M388" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="389" spans="1:13" x14ac:dyDescent="0.2">
@@ -16699,10 +16693,10 @@
         <v>59</v>
       </c>
       <c r="L389" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M389" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.2">
@@ -16740,10 +16734,10 @@
         <v>59</v>
       </c>
       <c r="L390" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M390" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="391" spans="1:13" x14ac:dyDescent="0.2">
@@ -16781,10 +16775,10 @@
         <v>59</v>
       </c>
       <c r="L391" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M391" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="392" spans="1:13" x14ac:dyDescent="0.2">
@@ -16822,10 +16816,10 @@
         <v>59</v>
       </c>
       <c r="L392" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M392" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="393" spans="1:13" x14ac:dyDescent="0.2">
@@ -16863,10 +16857,10 @@
         <v>59</v>
       </c>
       <c r="L393" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M393" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="394" spans="1:13" x14ac:dyDescent="0.2">
@@ -16904,10 +16898,10 @@
         <v>59</v>
       </c>
       <c r="L394" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M394" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="395" spans="1:13" x14ac:dyDescent="0.2">
@@ -16945,10 +16939,10 @@
         <v>59</v>
       </c>
       <c r="L395" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M395" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="396" spans="1:13" x14ac:dyDescent="0.2">
@@ -16986,10 +16980,10 @@
         <v>59</v>
       </c>
       <c r="L396" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M396" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="397" spans="1:13" x14ac:dyDescent="0.2">
@@ -17027,10 +17021,10 @@
         <v>59</v>
       </c>
       <c r="L397" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M397" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="398" spans="1:13" x14ac:dyDescent="0.2">
@@ -17068,10 +17062,10 @@
         <v>59</v>
       </c>
       <c r="L398" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M398" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="399" spans="1:13" x14ac:dyDescent="0.2">
@@ -17109,10 +17103,10 @@
         <v>59</v>
       </c>
       <c r="L399" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M399" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="400" spans="1:13" x14ac:dyDescent="0.2">
@@ -17150,10 +17144,10 @@
         <v>59</v>
       </c>
       <c r="L400" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M400" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="401" spans="1:13" x14ac:dyDescent="0.2">
@@ -17191,10 +17185,10 @@
         <v>59</v>
       </c>
       <c r="L401" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M401" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="402" spans="1:13" x14ac:dyDescent="0.2">
@@ -17232,10 +17226,10 @@
         <v>59</v>
       </c>
       <c r="L402" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M402" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="403" spans="1:13" x14ac:dyDescent="0.2">
@@ -17273,10 +17267,10 @@
         <v>59</v>
       </c>
       <c r="L403" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M403" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="404" spans="1:13" x14ac:dyDescent="0.2">
@@ -17314,10 +17308,10 @@
         <v>59</v>
       </c>
       <c r="L404" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M404" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="405" spans="1:13" x14ac:dyDescent="0.2">
@@ -17355,10 +17349,10 @@
         <v>59</v>
       </c>
       <c r="L405" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M405" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="406" spans="1:13" x14ac:dyDescent="0.2">
@@ -17396,10 +17390,10 @@
         <v>59</v>
       </c>
       <c r="L406" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M406" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>